<commit_message>
Deploy to test server
</commit_message>
<xml_diff>
--- a/dev/v8web/src/main/resources/static/xls/compliance_control.xlsx
+++ b/dev/v8web/src/main/resources/static/xls/compliance_control.xlsx
@@ -234,7 +234,7 @@
     <t xml:space="preserve">if count(*) &gt; 0, then child labor, which is not ok: indicator not validated</t>
   </si>
   <si>
-    <t xml:space="preserve">Sanitary facilities - Access to toilet</t>
+    <t xml:space="preserve">Sanitary facilities – No Access to toilet</t>
   </si>
   <si>
     <r>
@@ -298,17 +298,17 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFDDDDDD"/>
-        <rFont val="Monospace"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">reg_entities;</t>
+      <t xml:space="preserve"> reg_entity_farmaq_details</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFDDDDDD"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">;</t>
     </r>
   </si>
   <si>
@@ -318,7 +318,7 @@
     <t xml:space="preserve">yes= compliance / No (or not defined) = no compliance</t>
   </si>
   <si>
-    <t xml:space="preserve">Access to toilet</t>
+    <t xml:space="preserve">crash test</t>
   </si>
   <si>
     <r>
@@ -602,13 +602,13 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="52.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="64.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.14"/>

</xml_diff>

<commit_message>
Set true at 1 and false at 0 on compliance.
</commit_message>
<xml_diff>
--- a/dev/v8web/src/main/resources/static/xls/compliance_control.xlsx
+++ b/dev/v8web/src/main/resources/static/xls/compliance_control.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">Standard name</t>
   </si>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Comment</t>
   </si>
   <si>
-    <t xml:space="preserve">Child labor</t>
+    <t xml:space="preserve">NO Child labor</t>
   </si>
   <si>
     <r>
@@ -62,6 +62,7 @@
     </r>
     <r>
       <rPr>
+        <b val="true"/>
         <sz val="10"/>
         <color rgb="FF839496"/>
         <rFont val="Monospace"/>
@@ -79,10 +80,11 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">COUNT</t>
-    </r>
-    <r>
-      <rPr>
+      <t xml:space="preserve">count</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
         <sz val="10"/>
         <color rgb="FFDDDDDD"/>
         <rFont val="Monospace"/>
@@ -93,6 +95,7 @@
     </r>
     <r>
       <rPr>
+        <b val="true"/>
         <sz val="10"/>
         <color rgb="FF839496"/>
         <rFont val="Monospace"/>
@@ -110,20 +113,198 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">FROM</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF839496"/>
-        <rFont val="Monospace"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
+      <t xml:space="preserve">from</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF839496"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFDDDDDD"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">reg_entities</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF839496"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF8040"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">where</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF839496"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFDDDDDD"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ID</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF839496"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF8040"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">in</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF839496"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFDDDDDD"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF839496"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF8040"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">select</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF839496"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFDDDDDD"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">reg_entity_id</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF839496"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF8040"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">from</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF839496"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
         <sz val="10"/>
         <color rgb="FFDDDDDD"/>
         <rFont val="Monospace"/>
@@ -134,6 +315,7 @@
     </r>
     <r>
       <rPr>
+        <b val="true"/>
         <sz val="10"/>
         <color rgb="FF839496"/>
         <rFont val="Monospace"/>
@@ -151,60 +333,33 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">WHERE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF839496"/>
-        <rFont val="Monospace"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFDDDDDD"/>
-        <rFont val="Monospace"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">REG_ENTITY_FARM_ID</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF839496"/>
-        <rFont val="Monospace"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFDDDDDD"/>
-        <rFont val="Monospace"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF839496"/>
-        <rFont val="Monospace"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
+      <t xml:space="preserve">where</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF839496"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFDDDDDD"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">reg_entity_farm_id=</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
         <sz val="10"/>
         <color rgb="FF008080"/>
         <rFont val="Monospace"/>
@@ -215,8 +370,229 @@
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
-        <color rgb="FFDDDDDD"/>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFDDDDDD"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF839496"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF8040"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">and</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF839496"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFDDDDDD"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF8040"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">YEAR</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFDDDDDD"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(DATE_OF_BIRTH)</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF839496"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFDDDDDD"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF839496"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFF8040"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">YEAR</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFDDDDDD"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFFFFF80"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">NOW</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFDDDDDD"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">())</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF839496"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFDDDDDD"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF839496"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF008080"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">18</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF839496"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FFDDDDDD"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <color rgb="FF839496"/>
         <rFont val="Monospace"/>
         <family val="0"/>
         <charset val="1"/>
@@ -228,175 +604,22 @@
     <t xml:space="preserve">numeric</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;</t>
+    <t xml:space="preserve">&lt;=</t>
   </si>
   <si>
     <t xml:space="preserve">if count(*) &gt; 0, then child labor, which is not ok: indicator not validated</t>
   </si>
   <si>
-    <t xml:space="preserve">Sanitary facilities – No Access to toilet</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color rgb="FFFF8040"/>
-        <rFont val="Monospace"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">SELECT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF839496"/>
-        <rFont val="Monospace"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color rgb="FFFFFF80"/>
-        <rFont val="Monospace"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">COUNT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFDDDDDD"/>
-        <rFont val="Monospace"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(*) </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color rgb="FFFF8040"/>
-        <rFont val="Monospace"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">FROM</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF839496"/>
-        <rFont val="Monospace"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> reg_entity_farmaq_details</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFDDDDDD"/>
-        <rFont val="Monospace"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">;</t>
-    </r>
+    <t xml:space="preserve">Sanitary facilities – Access to toilet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT ACCESS_TOILETS FROM reg_entity_facilities WHERE REG_ENTITY_FARM_ID = {ID};</t>
   </si>
   <si>
     <t xml:space="preserve">boolean</t>
   </si>
   <si>
     <t xml:space="preserve">yes= compliance / No (or not defined) = no compliance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">crash test</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color rgb="FFFF8040"/>
-        <rFont val="Monospace"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">SELECT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF839496"/>
-        <rFont val="Monospace"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color rgb="FFFFFF80"/>
-        <rFont val="Monospace"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">COUNT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFDDDDDD"/>
-        <rFont val="Monospace"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(*) </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <color rgb="FFFF8040"/>
-        <rFont val="Monospace"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">FROM</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF839496"/>
-        <rFont val="Monospace"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFDDDDDD"/>
-        <rFont val="Monospace"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">reg_entity;</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Failed testing</t>
   </si>
 </sst>
 </file>
@@ -438,6 +661,7 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FF839496"/>
       <name val="Monospace"/>
@@ -453,6 +677,7 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FFDDDDDD"/>
       <name val="Monospace"/>
@@ -460,6 +685,7 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FF008080"/>
       <name val="Monospace"/>
@@ -599,10 +825,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -656,7 +882,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>11</v>
@@ -679,20 +905,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>